<commit_message>
clean up for publication
</commit_message>
<xml_diff>
--- a/figures_and_tables/table2/interaction_parameters_data.xlsx
+++ b/figures_and_tables/table2/interaction_parameters_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimda\Documents\PhD_Local\3-Repositories\PendantProp\data\mixture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pimda\Documents\PhD_Local\3-Repositories\PendantProp\figures_and_tables\table2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38F21D2-ACCF-4D40-9A0E-417D5334DF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97680CD5-9961-4962-9C5A-C81F78A002E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60120" yWindow="-5475" windowWidth="21840" windowHeight="37920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -157,7 +157,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +474,7 @@
         <v>-2.2999999999999998</v>
       </c>
       <c r="D2" s="1">
-        <v>-1.1499999999999999</v>
+        <v>-1.1000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -485,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>-1.2</v>

</xml_diff>